<commit_message>
check all elemenets // resolve some troubles
</commit_message>
<xml_diff>
--- a/Design system for Darkroom.xlsx
+++ b/Design system for Darkroom.xlsx
@@ -11,27 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="159">
-  <si>
-    <t>Custop Prop</t>
-  </si>
-  <si>
-    <t>Color #</t>
-  </si>
-  <si>
-    <t>Dark-Mode</t>
-  </si>
-  <si>
-    <t>--back-color</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="158">
+  <si>
+    <t>Index / body / backcolor</t>
   </si>
   <si>
     <t>#FFFFFF</t>
   </si>
   <si>
-    <t>#060A0F</t>
-  </si>
-  <si>
-    <t>INDEX</t>
+    <t>#060A0F !important</t>
+  </si>
+  <si>
+    <t>—body-changes</t>
   </si>
   <si>
     <t>index / body / title</t>
@@ -43,9 +34,24 @@
     <t>—topic-title-grey</t>
   </si>
   <si>
+    <t>#E6E6E6</t>
+  </si>
+  <si>
+    <t>#35393F</t>
+  </si>
+  <si>
+    <t>—border-grey</t>
+  </si>
+  <si>
     <t>index / body / description</t>
   </si>
   <si>
+    <t>#ECECEC</t>
+  </si>
+  <si>
+    <t>—bottom-grey</t>
+  </si>
+  <si>
     <t>index / create-button / backcolor</t>
   </si>
   <si>
@@ -58,6 +64,12 @@
     <t>—pastel-green</t>
   </si>
   <si>
+    <t>#3B424B</t>
+  </si>
+  <si>
+    <t>—comment-grey</t>
+  </si>
+  <si>
     <t>index / create-button / backcolor / hover</t>
   </si>
   <si>
@@ -67,19 +79,31 @@
     <t>—middle-green</t>
   </si>
   <si>
+    <t>#1B1B1B</t>
+  </si>
+  <si>
+    <t>—dark-mode-yellow</t>
+  </si>
+  <si>
     <t>1.HEADER</t>
   </si>
   <si>
+    <t>#222222</t>
+  </si>
+  <si>
+    <t>—darkmode-bottom-black</t>
+  </si>
+  <si>
     <t>header / border-bottom</t>
   </si>
   <si>
-    <t>#ECECEC</t>
-  </si>
-  <si>
-    <t>#35393F</t>
-  </si>
-  <si>
-    <t>—bottom-grey</t>
+    <t>#FEFF9B</t>
+  </si>
+  <si>
+    <t>#242424</t>
+  </si>
+  <si>
+    <t>—darkmode-text-white</t>
   </si>
   <si>
     <t>header / backcolor</t>
@@ -100,16 +124,28 @@
     <t>—middle-grey</t>
   </si>
   <si>
+    <t>#CCCCCC</t>
+  </si>
+  <si>
+    <t>—link-footer-green</t>
+  </si>
+  <si>
     <t>menu-login / border</t>
   </si>
   <si>
+    <t>#77CFB2</t>
+  </si>
+  <si>
+    <t>—link-hover-green</t>
+  </si>
+  <si>
     <t>dark-mode-button / color</t>
   </si>
   <si>
-    <t>#1B1B1B</t>
-  </si>
-  <si>
-    <t>—dark-mode-yellow</t>
+    <t>#676767</t>
+  </si>
+  <si>
+    <t>—list-grey</t>
   </si>
   <si>
     <t>dark-mode-button / backcolor</t>
@@ -118,24 +154,12 @@
     <t>dark-mode-button / hover / backcolor</t>
   </si>
   <si>
-    <t>#222222</t>
-  </si>
-  <si>
-    <t>—darkmode-bottom-black</t>
+    <t>—middle-green-link</t>
   </si>
   <si>
     <t>dark-mode-button / hover / color</t>
   </si>
   <si>
-    <t>#FEFF9B</t>
-  </si>
-  <si>
-    <t>#242424</t>
-  </si>
-  <si>
-    <t>—darkmode-text-white</t>
-  </si>
-  <si>
     <t>dark-mode-button / back-image</t>
   </si>
   <si>
@@ -145,51 +169,84 @@
     <t>url(../Media/Sun.png)</t>
   </si>
   <si>
+    <t>#333333</t>
+  </si>
+  <si>
+    <t>—opacity-color</t>
+  </si>
+  <si>
     <t>menu-underlined / after</t>
   </si>
   <si>
     <t>menu-login / hover / color</t>
   </si>
   <si>
+    <t>#52AA91</t>
+  </si>
+  <si>
+    <t>—podcast-green</t>
+  </si>
+  <si>
     <t>meni-login / hover / border</t>
   </si>
   <si>
+    <t>rgba(0,0,0,0.27)</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>—quote-text-before</t>
+  </si>
+  <si>
     <t>menu-gallery / backcolor</t>
   </si>
   <si>
+    <t>linear-gradient(to top right, rgb(77, 85, 92), rgb(211, 211, 211));</t>
+  </si>
+  <si>
+    <t>linear-gradient(to top right, rgb(36, 39, 43), rgb(211, 211, 211));</t>
+  </si>
+  <si>
+    <t>—screen-gradient</t>
+  </si>
+  <si>
     <t>menu-login / color</t>
   </si>
   <si>
+    <t>#F1F1F1</t>
+  </si>
+  <si>
+    <t>—square-template-grey</t>
+  </si>
+  <si>
+    <t>#444444</t>
+  </si>
+  <si>
+    <t>—title-text-grey</t>
+  </si>
+  <si>
     <t>2.FIRST SCREEN</t>
   </si>
   <si>
     <t>screen-container / after / backimage</t>
   </si>
   <si>
-    <t>linear-gradient(to top right, rgb(77, 85, 92), rgb(211, 211, 211));</t>
-  </si>
-  <si>
-    <t>linear-gradient(to top right, rgb(36, 39, 43), rgb(211, 211, 211));</t>
-  </si>
-  <si>
-    <t>—screen-gradient</t>
+    <t>—underline-green</t>
   </si>
   <si>
     <t>posotion-button / backcolor</t>
   </si>
   <si>
+    <t>—viewallpost-green</t>
+  </si>
+  <si>
     <t>3.WORKBLOCK</t>
   </si>
   <si>
     <t>workblock-container-picture-pic / backcolor</t>
   </si>
   <si>
-    <t>#F1F1F1</t>
-  </si>
-  <si>
-    <t>—square-template-grey</t>
-  </si>
-  <si>
     <t>workblock-container-picture-pic / before / backimage</t>
   </si>
   <si>
@@ -211,12 +268,6 @@
     <t>h6 / color</t>
   </si>
   <si>
-    <t>#444444</t>
-  </si>
-  <si>
-    <t>—title-text-grey</t>
-  </si>
-  <si>
     <t>p / color</t>
   </si>
   <si>
@@ -247,12 +298,6 @@
     <t>li / color</t>
   </si>
   <si>
-    <t>#676767</t>
-  </si>
-  <si>
-    <t>—list-grey</t>
-  </si>
-  <si>
     <t>li / after / backimage</t>
   </si>
   <si>
@@ -316,60 +361,27 @@
     <t>quote-text / backcolor</t>
   </si>
   <si>
-    <t>#3B424B</t>
-  </si>
-  <si>
-    <t>—comment-grey</t>
-  </si>
-  <si>
     <t>Quote-arrow / backcolor</t>
   </si>
   <si>
     <t>quote-text / before</t>
   </si>
   <si>
-    <t>rgba(0,0,0,0.27)</t>
-  </si>
-  <si>
-    <t>#000000</t>
-  </si>
-  <si>
-    <t>—quote-text-before</t>
-  </si>
-  <si>
     <t>8.ITEMS BLOCK</t>
   </si>
   <si>
-    <t>Item-oe / before / backcolor</t>
-  </si>
-  <si>
-    <t>#333333</t>
-  </si>
-  <si>
-    <t>—opacity-color</t>
+    <t>Item-oe / after / backcolor</t>
   </si>
   <si>
     <t>Item-ue / after / backcolor</t>
   </si>
   <si>
-    <t>#52AA91</t>
-  </si>
-  <si>
-    <t>—underline-green</t>
-  </si>
-  <si>
     <t>9.DARKROOM</t>
   </si>
   <si>
     <t>Darkroom-container-style / border</t>
   </si>
   <si>
-    <t>#E6E6E6</t>
-  </si>
-  <si>
-    <t>—border-grey</t>
-  </si>
-  <si>
     <t>Darkroom-container-style / before / backcolor</t>
   </si>
   <si>
@@ -415,9 +427,6 @@
     <t>Link / hover / border</t>
   </si>
   <si>
-    <t>—podcast-green</t>
-  </si>
-  <si>
     <t>Link / hover / backcolor</t>
   </si>
   <si>
@@ -439,9 +448,6 @@
     <t>View-all-posts / hover / backcolor</t>
   </si>
   <si>
-    <t>—viewallpost-green</t>
-  </si>
-  <si>
     <t xml:space="preserve">View-all-posts / p / color </t>
   </si>
   <si>
@@ -472,22 +478,13 @@
     <t>A / color</t>
   </si>
   <si>
-    <t>#CCCCCC</t>
-  </si>
-  <si>
-    <t>—link-footer-green</t>
+    <t>—link-footer-grey</t>
   </si>
   <si>
     <t>Opacity</t>
   </si>
   <si>
     <t>A / hover / color</t>
-  </si>
-  <si>
-    <t>#77CFB2</t>
-  </si>
-  <si>
-    <t>—link-hover-green</t>
   </si>
 </sst>
 </file>
@@ -497,7 +494,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -511,13 +508,7 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="4">
@@ -569,7 +560,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -586,12 +577,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -617,9 +602,9 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffcde7ea"/>
+      <rgbColor rgb="ffcdd8fa"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffe7f3f4"/>
+      <rgbColor rgb="ffe7ecfc"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -818,12 +803,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -856,10 +841,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1107,12 +1092,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1427,10 +1412,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1690,13 +1675,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="11.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="41.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="48.4219" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6484" style="1" customWidth="1"/>
+    <col min="1" max="1" width="41.8516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7656" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7969" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6719" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27" style="1" customWidth="1"/>
-    <col min="7" max="13" width="14.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.9844" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109" style="1" customWidth="1"/>
+    <col min="9" max="13" width="14.5" style="1" customWidth="1"/>
     <col min="14" max="256" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1725,7 +1712,9 @@
       <c r="C2" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" t="s" s="3">
+        <v>3</v>
+      </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1738,19 +1727,27 @@
     </row>
     <row r="3" ht="11.65" customHeight="1">
       <c r="A3" t="s" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D3" t="s" s="5">
+        <v>6</v>
+      </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="F3" t="s" s="5">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s" s="5">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s" s="5">
+        <v>9</v>
+      </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1758,14 +1755,28 @@
       <c r="M3" s="2"/>
     </row>
     <row r="4" ht="11.65" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="A4" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s" s="3">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s" s="3">
+        <v>6</v>
+      </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="F4" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s" s="3">
+        <v>12</v>
+      </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -1773,14 +1784,28 @@
       <c r="M4" s="4"/>
     </row>
     <row r="5" ht="11.65" customHeight="1">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="A5" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s" s="5">
+        <v>16</v>
+      </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="F5" t="s" s="5">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s" s="5">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s" s="5">
+        <v>18</v>
+      </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1788,14 +1813,28 @@
       <c r="M5" s="2"/>
     </row>
     <row r="6" ht="11.65" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="A6" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s" s="3">
+        <v>21</v>
+      </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="F6" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s" s="3">
+        <v>23</v>
+      </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -1803,14 +1842,22 @@
       <c r="M6" s="4"/>
     </row>
     <row r="7" ht="11.65" customHeight="1">
-      <c r="A7" s="2"/>
+      <c r="A7" t="s" s="5">
+        <v>24</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="F7" t="s" s="5">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s" s="5">
+        <v>26</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1818,14 +1865,28 @@
       <c r="M7" s="2"/>
     </row>
     <row r="8" ht="11.65" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="A8" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s" s="3">
+        <v>12</v>
+      </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="F8" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="G8" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="H8" t="s" s="3">
+        <v>30</v>
+      </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -1833,14 +1894,28 @@
       <c r="M8" s="4"/>
     </row>
     <row r="9" ht="11.65" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="A9" t="s" s="5">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s" s="5">
+        <v>33</v>
+      </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="F9" t="s" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="H9" t="s" s="5">
+        <v>33</v>
+      </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -1848,14 +1923,28 @@
       <c r="M9" s="2"/>
     </row>
     <row r="10" ht="11.65" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="A10" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s" s="3">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s" s="3">
+        <v>36</v>
+      </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="F10" t="s" s="3">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s" s="3">
+        <v>38</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -1863,14 +1952,28 @@
       <c r="M10" s="4"/>
     </row>
     <row r="11" ht="11.65" customHeight="1">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="A11" t="s" s="5">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s" s="5">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s" s="5">
+        <v>36</v>
+      </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="F11" t="s" s="5">
+        <v>40</v>
+      </c>
+      <c r="G11" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s" s="5">
+        <v>41</v>
+      </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1878,16 +1981,28 @@
       <c r="M11" s="2"/>
     </row>
     <row r="12" ht="11.65" customHeight="1">
-      <c r="A12" t="s" s="6">
-        <v>6</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="A12" t="s" s="3">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s" s="3">
+        <v>23</v>
+      </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="F12" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="G12" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s" s="3">
+        <v>44</v>
+      </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -1896,21 +2011,27 @@
     </row>
     <row r="13" ht="11.65" customHeight="1">
       <c r="A13" t="s" s="5">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s" s="5">
         <v>8</v>
       </c>
-      <c r="C13" t="s" s="5">
-        <v>4</v>
-      </c>
       <c r="D13" t="s" s="5">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="F13" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="H13" t="s" s="5">
+        <v>21</v>
+      </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -1919,21 +2040,27 @@
     </row>
     <row r="14" ht="11.65" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s" s="3">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="F14" t="s" s="3">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s" s="3">
+        <v>47</v>
+      </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -1942,21 +2069,27 @@
     </row>
     <row r="15" ht="11.65" customHeight="1">
       <c r="A15" t="s" s="5">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s" s="5">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s" s="5">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s" s="5">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="F15" t="s" s="5">
+        <v>35</v>
+      </c>
+      <c r="G15" t="s" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s" s="5">
+        <v>36</v>
+      </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1965,21 +2098,25 @@
     </row>
     <row r="16" ht="11.65" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s" s="3">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s" s="3">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s" s="3">
-        <v>17</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="F16" t="s" s="3">
+        <v>52</v>
+      </c>
+      <c r="G16" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="H16" t="s" s="3">
+        <v>53</v>
+      </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -1987,16 +2124,28 @@
       <c r="M16" s="4"/>
     </row>
     <row r="17" ht="11.65" customHeight="1">
-      <c r="A17" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="A17" t="s" s="5">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s" s="5">
+        <v>21</v>
+      </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="F17" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s" s="5">
+        <v>16</v>
+      </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -2005,21 +2154,27 @@
     </row>
     <row r="18" ht="11.65" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s" s="3">
         <v>20</v>
       </c>
       <c r="C18" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="D18" t="s" s="3">
-        <v>22</v>
-      </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="F18" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s" s="3">
+        <v>56</v>
+      </c>
+      <c r="H18" t="s" s="3">
+        <v>57</v>
+      </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -2028,21 +2183,27 @@
     </row>
     <row r="19" ht="11.65" customHeight="1">
       <c r="A19" t="s" s="5">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s" s="5">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s" s="5">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s" s="5">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="F19" t="s" s="5">
+        <v>59</v>
+      </c>
+      <c r="G19" t="s" s="5">
+        <v>60</v>
+      </c>
+      <c r="H19" t="s" s="5">
+        <v>61</v>
+      </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -2051,21 +2212,27 @@
     </row>
     <row r="20" ht="11.65" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s" s="3">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s" s="3">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s" s="3">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="F20" t="s" s="3">
+        <v>63</v>
+      </c>
+      <c r="G20" t="s" s="3">
+        <v>64</v>
+      </c>
+      <c r="H20" t="s" s="3">
+        <v>65</v>
+      </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -2074,21 +2241,27 @@
     </row>
     <row r="21" ht="11.65" customHeight="1">
       <c r="A21" t="s" s="5">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s" s="5">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s" s="5">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="F21" t="s" s="5">
+        <v>67</v>
+      </c>
+      <c r="G21" t="s" s="5">
+        <v>8</v>
+      </c>
+      <c r="H21" t="s" s="5">
+        <v>68</v>
+      </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -2097,21 +2270,27 @@
     </row>
     <row r="22" ht="11.65" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s" s="3">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s" s="3">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="F22" t="s" s="3">
+        <v>69</v>
+      </c>
+      <c r="G22" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s" s="3">
+        <v>70</v>
+      </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -2120,21 +2299,21 @@
     </row>
     <row r="23" ht="11.65" customHeight="1">
       <c r="A23" t="s" s="5">
-        <v>33</v>
-      </c>
-      <c r="B23" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="C23" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="D23" t="s" s="5">
-        <v>22</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="F23" t="s" s="5">
+        <v>5</v>
+      </c>
+      <c r="G23" t="s" s="5">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s" s="5">
+        <v>6</v>
+      </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -2143,21 +2322,27 @@
     </row>
     <row r="24" ht="11.65" customHeight="1">
       <c r="A24" t="s" s="3">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s" s="3">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s" s="3">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="D24" t="s" s="3">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="F24" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="G24" t="s" s="3">
+        <v>56</v>
+      </c>
+      <c r="H24" t="s" s="3">
+        <v>73</v>
+      </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -2166,21 +2351,27 @@
     </row>
     <row r="25" ht="11.65" customHeight="1">
       <c r="A25" t="s" s="5">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s" s="5">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s" s="5">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D25" t="s" s="5">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="F25" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="G25" t="s" s="5">
+        <v>56</v>
+      </c>
+      <c r="H25" t="s" s="5">
+        <v>75</v>
+      </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -2189,14 +2380,10 @@
     </row>
     <row r="26" ht="11.65" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>41</v>
-      </c>
-      <c r="B26" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="C26" t="s" s="3">
-        <v>43</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -2210,16 +2397,16 @@
     </row>
     <row r="27" ht="11.65" customHeight="1">
       <c r="A27" t="s" s="5">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s" s="5">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s" s="5">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s" s="5">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -2233,17 +2420,15 @@
     </row>
     <row r="28" ht="11.65" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s" s="3">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s" s="3">
-        <v>13</v>
-      </c>
-      <c r="D28" t="s" s="3">
-        <v>17</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -2256,17 +2441,15 @@
     </row>
     <row r="29" ht="11.65" customHeight="1">
       <c r="A29" t="s" s="5">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s" s="5">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s" s="5">
-        <v>13</v>
-      </c>
-      <c r="D29" t="s" s="5">
-        <v>17</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -2279,16 +2462,16 @@
     </row>
     <row r="30" ht="11.65" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s" s="3">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="C30" t="s" s="3">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s" s="3">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2302,16 +2485,16 @@
     </row>
     <row r="31" ht="11.65" customHeight="1">
       <c r="A31" t="s" s="5">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s" s="5">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D31" t="s" s="5">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -2325,17 +2508,11 @@
     </row>
     <row r="32" ht="11.65" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>29</v>
-      </c>
-      <c r="B32" t="s" s="3">
-        <v>27</v>
-      </c>
-      <c r="C32" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s" s="3">
-        <v>28</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -2347,12 +2524,18 @@
       <c r="M32" s="4"/>
     </row>
     <row r="33" ht="11.65" customHeight="1">
-      <c r="A33" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="A33" t="s" s="5">
+        <v>87</v>
+      </c>
+      <c r="B33" t="s" s="5">
+        <v>67</v>
+      </c>
+      <c r="C33" t="s" s="5">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s" s="5">
+        <v>68</v>
+      </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -2365,17 +2548,15 @@
     </row>
     <row r="34" ht="11.65" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="B34" t="s" s="3">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="C34" t="s" s="3">
-        <v>52</v>
-      </c>
-      <c r="D34" t="s" s="3">
-        <v>53</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -2388,17 +2569,15 @@
     </row>
     <row r="35" ht="11.65" customHeight="1">
       <c r="A35" t="s" s="5">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s" s="5">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="C35" t="s" s="5">
-        <v>13</v>
-      </c>
-      <c r="D35" t="s" s="5">
-        <v>14</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -2410,12 +2589,18 @@
       <c r="M35" s="2"/>
     </row>
     <row r="36" ht="11.65" customHeight="1">
-      <c r="A36" t="s" s="6">
-        <v>55</v>
-      </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
+      <c r="A36" t="s" s="3">
+        <v>94</v>
+      </c>
+      <c r="B36" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s" s="3">
+        <v>44</v>
+      </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -2428,17 +2613,15 @@
     </row>
     <row r="37" ht="11.65" customHeight="1">
       <c r="A37" t="s" s="5">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="B37" t="s" s="5">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="D37" t="s" s="5">
-        <v>58</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -2451,13 +2634,13 @@
     </row>
     <row r="38" ht="11.65" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s" s="3">
-        <v>60</v>
-      </c>
-      <c r="C38" t="s" s="3">
-        <v>61</v>
+        <v>99</v>
+      </c>
+      <c r="C38" s="6">
+        <v>1</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -2472,14 +2655,10 @@
     </row>
     <row r="39" ht="11.65" customHeight="1">
       <c r="A39" t="s" s="5">
-        <v>62</v>
-      </c>
-      <c r="B39" t="s" s="5">
-        <v>63</v>
-      </c>
-      <c r="C39" t="s" s="5">
-        <v>64</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -2493,16 +2672,16 @@
     </row>
     <row r="40" ht="11.65" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="B40" t="s" s="3">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C40" t="s" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s" s="3">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -2516,17 +2695,15 @@
     </row>
     <row r="41" ht="11.65" customHeight="1">
       <c r="A41" t="s" s="5">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="B41" t="s" s="5">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="D41" t="s" s="5">
-        <v>67</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -2538,11 +2715,15 @@
       <c r="M41" s="2"/>
     </row>
     <row r="42" ht="11.65" customHeight="1">
-      <c r="A42" t="s" s="6">
-        <v>69</v>
-      </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
+      <c r="A42" t="s" s="3">
+        <v>105</v>
+      </c>
+      <c r="B42" t="s" s="3">
+        <v>106</v>
+      </c>
+      <c r="C42" t="s" s="3">
+        <v>107</v>
+      </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -2556,16 +2737,16 @@
     </row>
     <row r="43" ht="11.65" customHeight="1">
       <c r="A43" t="s" s="5">
+        <v>108</v>
+      </c>
+      <c r="B43" t="s" s="5">
+        <v>69</v>
+      </c>
+      <c r="C43" t="s" s="5">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s" s="5">
         <v>70</v>
-      </c>
-      <c r="B43" t="s" s="5">
-        <v>57</v>
-      </c>
-      <c r="C43" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="D43" t="s" s="5">
-        <v>58</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
@@ -2579,15 +2760,17 @@
     </row>
     <row r="44" ht="11.65" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B44" t="s" s="3">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C44" t="s" s="3">
-        <v>73</v>
-      </c>
-      <c r="D44" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="D44" t="s" s="3">
+        <v>70</v>
+      </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -2600,14 +2783,10 @@
     </row>
     <row r="45" ht="11.65" customHeight="1">
       <c r="A45" t="s" s="5">
-        <v>74</v>
-      </c>
-      <c r="B45" t="s" s="5">
-        <v>75</v>
-      </c>
-      <c r="C45" t="s" s="5">
-        <v>76</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
@@ -2621,16 +2800,16 @@
     </row>
     <row r="46" ht="11.65" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="B46" t="s" s="3">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C46" t="s" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D46" t="s" s="3">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -2644,13 +2823,13 @@
     </row>
     <row r="47" ht="11.65" customHeight="1">
       <c r="A47" t="s" s="5">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="B47" t="s" s="5">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="C47" t="s" s="5">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -2665,13 +2844,13 @@
     </row>
     <row r="48" ht="11.65" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="B48" t="s" s="3">
-        <v>84</v>
-      </c>
-      <c r="C48" s="8">
-        <v>1</v>
+        <v>112</v>
+      </c>
+      <c r="C48" t="s" s="3">
+        <v>113</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -2685,12 +2864,18 @@
       <c r="M48" s="4"/>
     </row>
     <row r="49" ht="11.65" customHeight="1">
-      <c r="A49" t="s" s="7">
-        <v>85</v>
-      </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+      <c r="A49" t="s" s="5">
+        <v>108</v>
+      </c>
+      <c r="B49" t="s" s="5">
+        <v>69</v>
+      </c>
+      <c r="C49" t="s" s="5">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s" s="5">
+        <v>70</v>
+      </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -2703,16 +2888,16 @@
     </row>
     <row r="50" ht="11.65" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s" s="3">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C50" t="s" s="3">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D50" t="s" s="3">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
@@ -2726,14 +2911,10 @@
     </row>
     <row r="51" ht="11.65" customHeight="1">
       <c r="A51" t="s" s="5">
-        <v>87</v>
-      </c>
-      <c r="B51" t="s" s="5">
-        <v>88</v>
-      </c>
-      <c r="C51" t="s" s="5">
-        <v>89</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
@@ -2747,15 +2928,17 @@
     </row>
     <row r="52" ht="11.65" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="B52" t="s" s="3">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="C52" t="s" s="3">
-        <v>92</v>
-      </c>
-      <c r="D52" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="D52" t="s" s="3">
+        <v>18</v>
+      </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -2768,16 +2951,16 @@
     </row>
     <row r="53" ht="11.65" customHeight="1">
       <c r="A53" t="s" s="5">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="B53" t="s" s="5">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="C53" t="s" s="5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D53" t="s" s="5">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
@@ -2791,16 +2974,16 @@
     </row>
     <row r="54" ht="11.65" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="B54" t="s" s="3">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C54" t="s" s="3">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="D54" t="s" s="3">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -2813,8 +2996,8 @@
       <c r="M54" s="4"/>
     </row>
     <row r="55" ht="11.65" customHeight="1">
-      <c r="A55" t="s" s="7">
-        <v>94</v>
+      <c r="A55" t="s" s="5">
+        <v>118</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2831,16 +3014,16 @@
     </row>
     <row r="56" ht="11.65" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="B56" t="s" s="3">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C56" t="s" s="3">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D56" t="s" s="3">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
@@ -2854,15 +3037,17 @@
     </row>
     <row r="57" ht="11.65" customHeight="1">
       <c r="A57" t="s" s="5">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="B57" t="s" s="5">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="C57" t="s" s="5">
-        <v>96</v>
-      </c>
-      <c r="D57" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="D57" t="s" s="5">
+        <v>73</v>
+      </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -2875,14 +3060,10 @@
     </row>
     <row r="58" ht="11.65" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>90</v>
-      </c>
-      <c r="B58" t="s" s="3">
-        <v>97</v>
-      </c>
-      <c r="C58" t="s" s="3">
-        <v>98</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -2896,16 +3077,16 @@
     </row>
     <row r="59" ht="11.65" customHeight="1">
       <c r="A59" t="s" s="5">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="B59" t="s" s="5">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="C59" t="s" s="5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D59" t="s" s="5">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
@@ -2919,16 +3100,16 @@
     </row>
     <row r="60" ht="11.65" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="B60" t="s" s="3">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C60" t="s" s="3">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D60" t="s" s="3">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
@@ -2941,12 +3122,18 @@
       <c r="M60" s="4"/>
     </row>
     <row r="61" ht="11.65" customHeight="1">
-      <c r="A61" t="s" s="7">
-        <v>99</v>
-      </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+      <c r="A61" t="s" s="5">
+        <v>124</v>
+      </c>
+      <c r="B61" t="s" s="5">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="D61" t="s" s="5">
+        <v>47</v>
+      </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -2959,16 +3146,16 @@
     </row>
     <row r="62" ht="11.65" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="B62" t="s" s="3">
-        <v>101</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s" s="3">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D62" t="s" s="3">
-        <v>102</v>
+        <v>6</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
@@ -2982,16 +3169,16 @@
     </row>
     <row r="63" ht="11.65" customHeight="1">
       <c r="A63" t="s" s="5">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="B63" t="s" s="5">
-        <v>101</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s" s="5">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D63" t="s" s="5">
-        <v>102</v>
+        <v>6</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
@@ -3005,17 +3192,15 @@
     </row>
     <row r="64" ht="11.65" customHeight="1">
       <c r="A64" t="s" s="3">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="B64" t="s" s="3">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="C64" t="s" s="3">
-        <v>106</v>
-      </c>
-      <c r="D64" t="s" s="3">
-        <v>107</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="D64" s="4"/>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -3027,11 +3212,15 @@
       <c r="M64" s="4"/>
     </row>
     <row r="65" ht="11.65" customHeight="1">
-      <c r="A65" t="s" s="7">
-        <v>108</v>
-      </c>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
+      <c r="A65" t="s" s="5">
+        <v>130</v>
+      </c>
+      <c r="B65" t="s" s="5">
+        <v>131</v>
+      </c>
+      <c r="C65" t="s" s="5">
+        <v>132</v>
+      </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
@@ -3045,16 +3234,16 @@
     </row>
     <row r="66" ht="11.65" customHeight="1">
       <c r="A66" t="s" s="3">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="B66" t="s" s="3">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="C66" t="s" s="3">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="D66" t="s" s="3">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
@@ -3068,16 +3257,16 @@
     </row>
     <row r="67" ht="11.65" customHeight="1">
       <c r="A67" t="s" s="5">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="B67" t="s" s="5">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="C67" t="s" s="5">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="D67" t="s" s="5">
-        <v>114</v>
+        <v>70</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
@@ -3090,11 +3279,15 @@
       <c r="M67" s="2"/>
     </row>
     <row r="68" ht="11.65" customHeight="1">
-      <c r="A68" t="s" s="6">
-        <v>115</v>
-      </c>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
+      <c r="A68" t="s" s="3">
+        <v>135</v>
+      </c>
+      <c r="B68" s="6">
+        <v>1</v>
+      </c>
+      <c r="C68" s="6">
+        <v>0.7</v>
+      </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
@@ -3108,17 +3301,11 @@
     </row>
     <row r="69" ht="11.65" customHeight="1">
       <c r="A69" t="s" s="5">
-        <v>116</v>
-      </c>
-      <c r="B69" t="s" s="5">
-        <v>117</v>
-      </c>
-      <c r="C69" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="D69" t="s" s="5">
-        <v>118</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
@@ -3131,16 +3318,16 @@
     </row>
     <row r="70" ht="11.65" customHeight="1">
       <c r="A70" t="s" s="3">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B70" t="s" s="3">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C70" t="s" s="3">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D70" t="s" s="3">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
@@ -3154,16 +3341,16 @@
     </row>
     <row r="71" ht="11.65" customHeight="1">
       <c r="A71" t="s" s="5">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="B71" t="s" s="5">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C71" t="s" s="5">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D71" t="s" s="5">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -3177,17 +3364,15 @@
     </row>
     <row r="72" ht="11.65" customHeight="1">
       <c r="A72" t="s" s="3">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="B72" t="s" s="3">
-        <v>8</v>
+        <v>140</v>
       </c>
       <c r="C72" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="D72" t="s" s="3">
-        <v>9</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="D72" s="4"/>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
@@ -3200,17 +3385,15 @@
     </row>
     <row r="73" ht="11.65" customHeight="1">
       <c r="A73" t="s" s="5">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="B73" t="s" s="5">
-        <v>8</v>
+        <v>142</v>
       </c>
       <c r="C73" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="D73" t="s" s="5">
-        <v>9</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
@@ -3223,15 +3406,17 @@
     </row>
     <row r="74" ht="11.65" customHeight="1">
       <c r="A74" t="s" s="3">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B74" t="s" s="3">
-        <v>124</v>
+        <v>5</v>
       </c>
       <c r="C74" t="s" s="3">
-        <v>125</v>
-      </c>
-      <c r="D74" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="D74" t="s" s="3">
+        <v>6</v>
+      </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
@@ -3247,12 +3432,14 @@
         <v>126</v>
       </c>
       <c r="B75" t="s" s="5">
-        <v>127</v>
+        <v>5</v>
       </c>
       <c r="C75" t="s" s="5">
-        <v>128</v>
-      </c>
-      <c r="D75" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D75" t="s" s="5">
+        <v>6</v>
+      </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
@@ -3265,16 +3452,16 @@
     </row>
     <row r="76" ht="11.65" customHeight="1">
       <c r="A76" t="s" s="3">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="B76" t="s" s="3">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="C76" t="s" s="3">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D76" t="s" s="3">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
@@ -3288,16 +3475,16 @@
     </row>
     <row r="77" ht="11.65" customHeight="1">
       <c r="A77" t="s" s="5">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="B77" t="s" s="5">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="C77" t="s" s="5">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D77" t="s" s="5">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -3311,15 +3498,17 @@
     </row>
     <row r="78" ht="11.65" customHeight="1">
       <c r="A78" t="s" s="3">
-        <v>131</v>
-      </c>
-      <c r="B78" s="8">
+        <v>145</v>
+      </c>
+      <c r="B78" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C78" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="D78" s="4"/>
+      <c r="C78" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="D78" t="s" s="3">
+        <v>70</v>
+      </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
@@ -3331,8 +3520,8 @@
       <c r="M78" s="4"/>
     </row>
     <row r="79" ht="11.65" customHeight="1">
-      <c r="A79" t="s" s="7">
-        <v>132</v>
+      <c r="A79" t="s" s="5">
+        <v>146</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -3349,16 +3538,16 @@
     </row>
     <row r="80" ht="11.65" customHeight="1">
       <c r="A80" t="s" s="3">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="B80" t="s" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C80" t="s" s="3">
-        <v>113</v>
+        <v>56</v>
       </c>
       <c r="D80" t="s" s="3">
-        <v>134</v>
+        <v>57</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
@@ -3372,17 +3561,15 @@
     </row>
     <row r="81" ht="11.65" customHeight="1">
       <c r="A81" t="s" s="5">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="B81" t="s" s="5">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="C81" t="s" s="5">
-        <v>113</v>
-      </c>
-      <c r="D81" t="s" s="5">
-        <v>134</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
@@ -3395,13 +3582,13 @@
     </row>
     <row r="82" ht="11.65" customHeight="1">
       <c r="A82" t="s" s="3">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="B82" t="s" s="3">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="C82" t="s" s="3">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
@@ -3416,13 +3603,13 @@
     </row>
     <row r="83" ht="11.65" customHeight="1">
       <c r="A83" t="s" s="5">
-        <v>138</v>
-      </c>
-      <c r="B83" t="s" s="5">
-        <v>139</v>
+        <v>152</v>
+      </c>
+      <c r="B83" s="7">
+        <v>1</v>
       </c>
       <c r="C83" t="s" s="5">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -3437,16 +3624,16 @@
     </row>
     <row r="84" ht="11.65" customHeight="1">
       <c r="A84" t="s" s="3">
-        <v>121</v>
+        <v>154</v>
       </c>
       <c r="B84" t="s" s="3">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C84" t="s" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D84" t="s" s="3">
-        <v>9</v>
+        <v>155</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
@@ -3460,17 +3647,15 @@
     </row>
     <row r="85" ht="11.65" customHeight="1">
       <c r="A85" t="s" s="5">
-        <v>122</v>
-      </c>
-      <c r="B85" t="s" s="5">
-        <v>8</v>
+        <v>156</v>
+      </c>
+      <c r="B85" s="7">
+        <v>1</v>
       </c>
       <c r="C85" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="D85" t="s" s="5">
-        <v>9</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="D85" s="2"/>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
@@ -3483,16 +3668,16 @@
     </row>
     <row r="86" ht="11.65" customHeight="1">
       <c r="A86" t="s" s="3">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="B86" t="s" s="3">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C86" t="s" s="3">
-        <v>113</v>
+        <v>15</v>
       </c>
       <c r="D86" t="s" s="3">
-        <v>134</v>
+        <v>41</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
@@ -3505,18 +3690,10 @@
       <c r="M86" s="4"/>
     </row>
     <row r="87" ht="11.65" customHeight="1">
-      <c r="A87" t="s" s="5">
-        <v>141</v>
-      </c>
-      <c r="B87" t="s" s="5">
-        <v>13</v>
-      </c>
-      <c r="C87" t="s" s="5">
-        <v>113</v>
-      </c>
-      <c r="D87" t="s" s="5">
-        <v>142</v>
-      </c>
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
@@ -3528,18 +3705,10 @@
       <c r="M87" s="2"/>
     </row>
     <row r="88" ht="11.65" customHeight="1">
-      <c r="A88" t="s" s="3">
-        <v>143</v>
-      </c>
-      <c r="B88" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C88" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="D88" t="s" s="3">
-        <v>67</v>
-      </c>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
@@ -3551,9 +3720,7 @@
       <c r="M88" s="4"/>
     </row>
     <row r="89" ht="11.65" customHeight="1">
-      <c r="A89" t="s" s="7">
-        <v>144</v>
-      </c>
+      <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
@@ -3568,18 +3735,10 @@
       <c r="M89" s="2"/>
     </row>
     <row r="90" ht="11.65" customHeight="1">
-      <c r="A90" t="s" s="3">
-        <v>145</v>
-      </c>
-      <c r="B90" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="C90" t="s" s="3">
-        <v>113</v>
-      </c>
-      <c r="D90" t="s" s="3">
-        <v>134</v>
-      </c>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
@@ -3591,15 +3750,9 @@
       <c r="M90" s="4"/>
     </row>
     <row r="91" ht="11.65" customHeight="1">
-      <c r="A91" t="s" s="5">
-        <v>146</v>
-      </c>
-      <c r="B91" t="s" s="5">
-        <v>84</v>
-      </c>
-      <c r="C91" t="s" s="5">
-        <v>147</v>
-      </c>
+      <c r="A91" s="2"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
@@ -3612,15 +3765,9 @@
       <c r="M91" s="2"/>
     </row>
     <row r="92" ht="11.65" customHeight="1">
-      <c r="A92" t="s" s="3">
-        <v>148</v>
-      </c>
-      <c r="B92" t="s" s="3">
-        <v>149</v>
-      </c>
-      <c r="C92" t="s" s="3">
-        <v>149</v>
-      </c>
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
@@ -3633,15 +3780,9 @@
       <c r="M92" s="4"/>
     </row>
     <row r="93" ht="11.65" customHeight="1">
-      <c r="A93" t="s" s="5">
-        <v>150</v>
-      </c>
-      <c r="B93" s="9">
-        <v>1</v>
-      </c>
-      <c r="C93" t="s" s="5">
-        <v>151</v>
-      </c>
+      <c r="A93" s="2"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
@@ -3654,18 +3795,10 @@
       <c r="M93" s="2"/>
     </row>
     <row r="94" ht="11.65" customHeight="1">
-      <c r="A94" t="s" s="3">
-        <v>152</v>
-      </c>
-      <c r="B94" t="s" s="3">
-        <v>153</v>
-      </c>
-      <c r="C94" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="D94" t="s" s="3">
-        <v>154</v>
-      </c>
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
@@ -3677,15 +3810,9 @@
       <c r="M94" s="4"/>
     </row>
     <row r="95" ht="11.65" customHeight="1">
-      <c r="A95" t="s" s="5">
-        <v>155</v>
-      </c>
-      <c r="B95" s="9">
-        <v>1</v>
-      </c>
-      <c r="C95" t="s" s="5">
-        <v>147</v>
-      </c>
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
@@ -3698,18 +3825,10 @@
       <c r="M95" s="2"/>
     </row>
     <row r="96" ht="11.65" customHeight="1">
-      <c r="A96" t="s" s="3">
-        <v>156</v>
-      </c>
-      <c r="B96" t="s" s="3">
-        <v>157</v>
-      </c>
-      <c r="C96" t="s" s="3">
-        <v>13</v>
-      </c>
-      <c r="D96" t="s" s="3">
-        <v>158</v>
-      </c>
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>

</xml_diff>

<commit_message>
cut off big part of JavaScript // resolve some troubles
</commit_message>
<xml_diff>
--- a/Design system for Darkroom.xlsx
+++ b/Design system for Darkroom.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="175">
   <si>
     <t>Index / body / backcolor</t>
   </si>
@@ -25,6 +25,9 @@
     <t>—body-changes</t>
   </si>
   <si>
+    <t>#AAAAAA</t>
+  </si>
+  <si>
     <t>index / body / title</t>
   </si>
   <si>
@@ -127,7 +130,7 @@
     <t>#CCCCCC</t>
   </si>
   <si>
-    <t>—link-footer-green</t>
+    <t>—link-footer-grey</t>
   </si>
   <si>
     <t>menu-login / border</t>
@@ -169,6 +172,9 @@
     <t>url(../Media/Sun.png)</t>
   </si>
   <si>
+    <t>—dark-mode-pic</t>
+  </si>
+  <si>
     <t>#333333</t>
   </si>
   <si>
@@ -256,6 +262,18 @@
     <t>url(../Media/1/1-dark.png)</t>
   </si>
   <si>
+    <t>—workblock-template-first-pic</t>
+  </si>
+  <si>
+    <t>url(../Media/10/author-na.png)</t>
+  </si>
+  <si>
+    <t>url(../Media/10/author-a.png)</t>
+  </si>
+  <si>
+    <t>—author-face-pic</t>
+  </si>
+  <si>
     <t>workblock-container-picture-pic / after / backimage</t>
   </si>
   <si>
@@ -265,39 +283,90 @@
     <t>url(../Media/1/2-dark.png)</t>
   </si>
   <si>
+    <t>—workblock-template-second-pic</t>
+  </si>
+  <si>
     <t>h6 / color</t>
   </si>
   <si>
+    <t>url(../Media/2/1.png)</t>
+  </si>
+  <si>
+    <t>url(../Media/2/1-dark.png)</t>
+  </si>
+  <si>
+    <t>—dashboard-template-first-pic</t>
+  </si>
+  <si>
     <t>p / color</t>
   </si>
   <si>
+    <t>url(../Media/2/2.jpg)</t>
+  </si>
+  <si>
+    <t>url(../Media/2/2-dark.png)</t>
+  </si>
+  <si>
+    <t>—dashboard-template-second-pic</t>
+  </si>
+  <si>
     <t>4.DASHBOARD</t>
   </si>
   <si>
+    <t>url(../Media/3/1.png)</t>
+  </si>
+  <si>
+    <t>url(../Media/3/1-dark.png)</t>
+  </si>
+  <si>
+    <t>—easypeasy-template-first-pic</t>
+  </si>
+  <si>
     <t>dashboard-container-picture-pic / backcolor</t>
   </si>
   <si>
+    <t>url(../Media/3/2.jpg)</t>
+  </si>
+  <si>
+    <t>url(../Media/3/2-dark.png)</t>
+  </si>
+  <si>
+    <t>—easypeasy-template-second-pic</t>
+  </si>
+  <si>
     <t>dashboard-container-picture-pic / before / backimage</t>
   </si>
   <si>
-    <t>url(../Media/2/1.png)</t>
-  </si>
-  <si>
-    <t>url(../Media/2/1-dark.png)</t>
+    <t>url(../Media/11/footer-back.png)</t>
+  </si>
+  <si>
+    <t>—footer-back-image</t>
   </si>
   <si>
     <t>dashboard-container-picture-pic / after / backimage</t>
   </si>
   <si>
-    <t>url(../Media/2/2.jpg)</t>
-  </si>
-  <si>
-    <t>url(../Media/2/2-dark.png)</t>
+    <t>url(../Media/9/basic-stack-01.png)</t>
+  </si>
+  <si>
+    <t>url(../Media/9/basic-stack-01-dark.png)</t>
+  </si>
+  <si>
+    <t>—free-template-pic</t>
   </si>
   <si>
     <t>li / color</t>
   </si>
   <si>
+    <t>url(../Media/9/pro-stack-01.png)</t>
+  </si>
+  <si>
+    <t>url(../Media/9/pro-stack-01-dark.png)</t>
+  </si>
+  <si>
+    <t>—plus-template-pic</t>
+  </si>
+  <si>
     <t>li / after / backimage</t>
   </si>
   <si>
@@ -307,12 +376,33 @@
     <t>url(../Media/2/done-dark.png)</t>
   </si>
   <si>
+    <t>—done</t>
+  </si>
+  <si>
+    <t>url(../Media/4/1.png)</t>
+  </si>
+  <si>
+    <t>url(../Media/4/1-dark.png)</t>
+  </si>
+  <si>
+    <t>—profits-template-first-pic</t>
+  </si>
+  <si>
     <t>li / after / opacity</t>
   </si>
   <si>
     <t>0.8</t>
   </si>
   <si>
+    <t>url(../Media/4/2.jpg)</t>
+  </si>
+  <si>
+    <t>url(../Media/4/2-dark.png)</t>
+  </si>
+  <si>
+    <t>—profits-template-second-pic</t>
+  </si>
+  <si>
     <t>5.EASYPEASYBLOCK</t>
   </si>
   <si>
@@ -322,37 +412,25 @@
     <t>easypeasy-container-picture-pic / before / backimage</t>
   </si>
   <si>
-    <t>url(../Media/3/1.png)</t>
-  </si>
-  <si>
-    <t>url(../Media/3/1-dark.png)</t>
+    <t>—done-pic</t>
   </si>
   <si>
     <t>easypeasy-container-picture-pic / after / backimage</t>
   </si>
   <si>
-    <t>url(../Media/3/2.jpg)</t>
-  </si>
-  <si>
-    <t>url(../Media/3/2-dark.png)</t>
-  </si>
-  <si>
     <t>h2 / color</t>
   </si>
   <si>
     <t>6.PROFITS DESERVE</t>
   </si>
   <si>
-    <t>url(../Media/4/1.png)</t>
-  </si>
-  <si>
-    <t>url(../Media/4/1-dark.png)</t>
-  </si>
-  <si>
-    <t>url(../Media/4/2.jpg)</t>
-  </si>
-  <si>
-    <t>url(../Media/4/2-dark.png)</t>
+    <t>profits-container-picture-pic / backcolor</t>
+  </si>
+  <si>
+    <t>profits-container-picture-pic / before / backimage</t>
+  </si>
+  <si>
+    <t>profits-container-picture-pic / after / backimage</t>
   </si>
   <si>
     <t>7.COMMENTS BLOCK</t>
@@ -397,21 +475,9 @@
     <t>Free / before / backimage</t>
   </si>
   <si>
-    <t>url(../Media/9/basic-stack-01.png)</t>
-  </si>
-  <si>
-    <t>url(../Media/9/basic-stack-01-dark.png)</t>
-  </si>
-  <si>
     <t>Plus / before / backimage</t>
   </si>
   <si>
-    <t>url(../Media/9/pro-stack-01.png)</t>
-  </si>
-  <si>
-    <t>url(../Media/9/pro-stack-01-dark.png)</t>
-  </si>
-  <si>
     <t>H4 / color</t>
   </si>
   <si>
@@ -433,15 +499,6 @@
     <t>Author / before / back image</t>
   </si>
   <si>
-    <t>url(../Media/10/author-na.png)</t>
-  </si>
-  <si>
-    <t>Author / hover / before / back image</t>
-  </si>
-  <si>
-    <t>url(../Media/10/author-a.png)</t>
-  </si>
-  <si>
     <t>View-all-posts / backcolor</t>
   </si>
   <si>
@@ -466,9 +523,6 @@
     <t>Ul / backimage</t>
   </si>
   <si>
-    <t>url(../Media/11/footer-back.png)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Opacity </t>
   </si>
   <si>
@@ -476,9 +530,6 @@
   </si>
   <si>
     <t>A / color</t>
-  </si>
-  <si>
-    <t>—link-footer-grey</t>
   </si>
   <si>
     <t>Opacity</t>
@@ -511,7 +562,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -527,6 +578,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="11"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -560,7 +617,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -579,7 +636,13 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -605,6 +668,7 @@
       <rgbColor rgb="ffcdd8fa"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffe7ecfc"/>
+      <rgbColor rgb="ff34a853"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1676,12 +1740,12 @@
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="11.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="41.8516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7656" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7969" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6719" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.2266" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.0312" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.0781" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.9844" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.3594" style="1" customWidth="1"/>
     <col min="8" max="8" width="25.7109" style="1" customWidth="1"/>
     <col min="9" max="13" width="14.5" style="1" customWidth="1"/>
     <col min="14" max="256" width="14.5" style="1" customWidth="1"/>
@@ -1716,9 +1780,15 @@
         <v>3</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="F2" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>3</v>
+      </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -1727,26 +1797,26 @@
     </row>
     <row r="3" ht="11.65" customHeight="1">
       <c r="A3" t="s" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s" s="5">
         <v>1</v>
       </c>
       <c r="D3" t="s" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1756,26 +1826,26 @@
     </row>
     <row r="4" ht="11.65" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s" s="3">
         <v>1</v>
       </c>
       <c r="D4" t="s" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" t="s" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H4" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -1785,26 +1855,26 @@
     </row>
     <row r="5" ht="11.65" customHeight="1">
       <c r="A5" t="s" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H5" t="s" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1814,26 +1884,26 @@
     </row>
     <row r="6" ht="11.65" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s" s="3">
         <v>1</v>
       </c>
       <c r="H6" t="s" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -1843,20 +1913,20 @@
     </row>
     <row r="7" ht="11.65" customHeight="1">
       <c r="A7" t="s" s="5">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" t="s" s="5">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s" s="5">
         <v>1</v>
       </c>
       <c r="H7" t="s" s="5">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1866,26 +1936,26 @@
     </row>
     <row r="8" ht="11.65" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" t="s" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H8" t="s" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1895,26 +1965,26 @@
     </row>
     <row r="9" ht="11.65" customHeight="1">
       <c r="A9" t="s" s="5">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s" s="5">
         <v>1</v>
       </c>
       <c r="C9" t="s" s="5">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s" s="5">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="5">
         <v>1</v>
       </c>
       <c r="G9" t="s" s="5">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H9" t="s" s="5">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1924,26 +1994,26 @@
     </row>
     <row r="10" ht="11.65" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s" s="3">
         <v>1</v>
       </c>
       <c r="D10" t="s" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" t="s" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G10" t="s" s="3">
         <v>1</v>
       </c>
       <c r="H10" t="s" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -1953,26 +2023,26 @@
     </row>
     <row r="11" ht="11.65" customHeight="1">
       <c r="A11" t="s" s="5">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s" s="5">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s" s="5">
         <v>1</v>
       </c>
       <c r="D11" t="s" s="5">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" t="s" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G11" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H11" t="s" s="5">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1982,26 +2052,26 @@
     </row>
     <row r="12" ht="11.65" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s" s="3">
         <v>1</v>
       </c>
       <c r="D12" t="s" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" t="s" s="3">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G12" t="s" s="3">
         <v>1</v>
       </c>
       <c r="H12" t="s" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -2011,26 +2081,26 @@
     </row>
     <row r="13" ht="11.65" customHeight="1">
       <c r="A13" t="s" s="5">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H13" t="s" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -2040,26 +2110,26 @@
     </row>
     <row r="14" ht="11.65" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s" s="3">
         <v>1</v>
       </c>
       <c r="D14" t="s" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G14" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H14" t="s" s="3">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -2069,26 +2139,26 @@
     </row>
     <row r="15" ht="11.65" customHeight="1">
       <c r="A15" t="s" s="5">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s" s="5">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s" s="5">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s" s="5">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" t="s" s="5">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G15" t="s" s="5">
         <v>1</v>
       </c>
       <c r="H15" t="s" s="5">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -2098,24 +2168,26 @@
     </row>
     <row r="16" ht="11.65" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s" s="3">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s" s="3">
-        <v>51</v>
-      </c>
-      <c r="D16" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="D16" t="s" s="6">
+        <v>53</v>
+      </c>
       <c r="E16" s="4"/>
       <c r="F16" t="s" s="3">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G16" t="s" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H16" t="s" s="3">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -2125,26 +2197,26 @@
     </row>
     <row r="17" ht="11.65" customHeight="1">
       <c r="A17" t="s" s="5">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G17" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H17" t="s" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -2154,26 +2226,26 @@
     </row>
     <row r="18" ht="11.65" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G18" t="s" s="3">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H18" t="s" s="3">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -2183,26 +2255,26 @@
     </row>
     <row r="19" ht="11.65" customHeight="1">
       <c r="A19" t="s" s="5">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" t="s" s="5">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G19" t="s" s="5">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H19" t="s" s="5">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -2212,26 +2284,26 @@
     </row>
     <row r="20" ht="11.65" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" t="s" s="3">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G20" t="s" s="3">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H20" t="s" s="3">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -2241,26 +2313,26 @@
     </row>
     <row r="21" ht="11.65" customHeight="1">
       <c r="A21" t="s" s="5">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s" s="5">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s" s="5">
         <v>1</v>
       </c>
       <c r="D21" t="s" s="5">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" t="s" s="5">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G21" t="s" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H21" t="s" s="5">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -2270,26 +2342,26 @@
     </row>
     <row r="22" ht="11.65" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s" s="3">
         <v>1</v>
       </c>
       <c r="D22" t="s" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" t="s" s="3">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G22" t="s" s="3">
         <v>1</v>
       </c>
       <c r="H22" t="s" s="3">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -2299,20 +2371,20 @@
     </row>
     <row r="23" ht="11.65" customHeight="1">
       <c r="A23" t="s" s="5">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" t="s" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G23" t="s" s="5">
         <v>1</v>
       </c>
       <c r="H23" t="s" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -2322,26 +2394,26 @@
     </row>
     <row r="24" ht="11.65" customHeight="1">
       <c r="A24" t="s" s="3">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s" s="3">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s" s="3">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s" s="3">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G24" t="s" s="3">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H24" t="s" s="3">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -2351,26 +2423,26 @@
     </row>
     <row r="25" ht="11.65" customHeight="1">
       <c r="A25" t="s" s="5">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D25" t="s" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G25" t="s" s="5">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H25" t="s" s="5">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2380,7 +2452,7 @@
     </row>
     <row r="26" ht="11.65" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2397,16 +2469,16 @@
     </row>
     <row r="27" ht="11.65" customHeight="1">
       <c r="A27" t="s" s="5">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s" s="5">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s" s="5">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -2420,19 +2492,27 @@
     </row>
     <row r="28" ht="11.65" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s" s="3">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s" s="3">
-        <v>80</v>
-      </c>
-      <c r="D28" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="D28" t="s" s="6">
+        <v>83</v>
+      </c>
       <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="F28" t="s" s="3">
+        <v>84</v>
+      </c>
+      <c r="G28" t="s" s="3">
+        <v>85</v>
+      </c>
+      <c r="H28" t="s" s="3">
+        <v>86</v>
+      </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -2441,19 +2521,27 @@
     </row>
     <row r="29" ht="11.65" customHeight="1">
       <c r="A29" t="s" s="5">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B29" t="s" s="5">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s" s="5">
-        <v>83</v>
-      </c>
-      <c r="D29" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="D29" t="s" s="6">
+        <v>90</v>
+      </c>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="F29" t="s" s="5">
+        <v>51</v>
+      </c>
+      <c r="G29" t="s" s="5">
+        <v>52</v>
+      </c>
+      <c r="H29" t="s" s="5">
+        <v>53</v>
+      </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
@@ -2462,21 +2550,27 @@
     </row>
     <row r="30" ht="11.65" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B30" t="s" s="3">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s" s="3">
         <v>1</v>
       </c>
       <c r="D30" t="s" s="3">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
+      <c r="F30" t="s" s="3">
+        <v>92</v>
+      </c>
+      <c r="G30" t="s" s="3">
+        <v>93</v>
+      </c>
+      <c r="H30" t="s" s="3">
+        <v>94</v>
+      </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -2485,21 +2579,27 @@
     </row>
     <row r="31" ht="11.65" customHeight="1">
       <c r="A31" t="s" s="5">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s" s="5">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s" s="5">
         <v>1</v>
       </c>
       <c r="D31" t="s" s="5">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+      <c r="F31" t="s" s="5">
+        <v>96</v>
+      </c>
+      <c r="G31" t="s" s="5">
+        <v>97</v>
+      </c>
+      <c r="H31" t="s" s="5">
+        <v>98</v>
+      </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -2508,15 +2608,21 @@
     </row>
     <row r="32" ht="11.65" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
+      <c r="F32" t="s" s="3">
+        <v>100</v>
+      </c>
+      <c r="G32" t="s" s="3">
+        <v>101</v>
+      </c>
+      <c r="H32" t="s" s="3">
+        <v>102</v>
+      </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -2525,21 +2631,27 @@
     </row>
     <row r="33" ht="11.65" customHeight="1">
       <c r="A33" t="s" s="5">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B33" t="s" s="5">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D33" t="s" s="5">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
+      <c r="F33" t="s" s="5">
+        <v>104</v>
+      </c>
+      <c r="G33" t="s" s="5">
+        <v>105</v>
+      </c>
+      <c r="H33" t="s" s="5">
+        <v>106</v>
+      </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
@@ -2548,19 +2660,27 @@
     </row>
     <row r="34" ht="11.65" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s" s="3">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C34" t="s" s="3">
-        <v>90</v>
-      </c>
-      <c r="D34" s="4"/>
+        <v>93</v>
+      </c>
+      <c r="D34" t="s" s="6">
+        <v>94</v>
+      </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
+      <c r="F34" t="s" s="3">
+        <v>108</v>
+      </c>
+      <c r="G34" t="s" s="3">
+        <v>108</v>
+      </c>
+      <c r="H34" t="s" s="3">
+        <v>109</v>
+      </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -2569,19 +2689,27 @@
     </row>
     <row r="35" ht="11.65" customHeight="1">
       <c r="A35" t="s" s="5">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="B35" t="s" s="5">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C35" t="s" s="5">
-        <v>93</v>
-      </c>
-      <c r="D35" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="D35" t="s" s="6">
+        <v>98</v>
+      </c>
       <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
+      <c r="F35" t="s" s="5">
+        <v>111</v>
+      </c>
+      <c r="G35" t="s" s="5">
+        <v>112</v>
+      </c>
+      <c r="H35" t="s" s="5">
+        <v>113</v>
+      </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -2590,21 +2718,27 @@
     </row>
     <row r="36" ht="11.65" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="B36" t="s" s="3">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s" s="3">
         <v>1</v>
       </c>
       <c r="D36" t="s" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
+      <c r="F36" t="s" s="3">
+        <v>115</v>
+      </c>
+      <c r="G36" t="s" s="3">
+        <v>116</v>
+      </c>
+      <c r="H36" t="s" s="3">
+        <v>117</v>
+      </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -2613,19 +2747,27 @@
     </row>
     <row r="37" ht="11.65" customHeight="1">
       <c r="A37" t="s" s="5">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="B37" t="s" s="5">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="C37" t="s" s="5">
-        <v>97</v>
-      </c>
-      <c r="D37" s="2"/>
+        <v>120</v>
+      </c>
+      <c r="D37" t="s" s="6">
+        <v>121</v>
+      </c>
       <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
+      <c r="F37" t="s" s="5">
+        <v>122</v>
+      </c>
+      <c r="G37" t="s" s="5">
+        <v>123</v>
+      </c>
+      <c r="H37" t="s" s="5">
+        <v>124</v>
+      </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
@@ -2634,19 +2776,25 @@
     </row>
     <row r="38" ht="11.65" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="B38" t="s" s="3">
-        <v>99</v>
-      </c>
-      <c r="C38" s="6">
+        <v>126</v>
+      </c>
+      <c r="C38" s="7">
         <v>1</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
+      <c r="F38" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="G38" t="s" s="3">
+        <v>128</v>
+      </c>
+      <c r="H38" t="s" s="3">
+        <v>129</v>
+      </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -2655,15 +2803,21 @@
     </row>
     <row r="39" ht="11.65" customHeight="1">
       <c r="A39" t="s" s="5">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
+      <c r="F39" t="s" s="5">
+        <v>81</v>
+      </c>
+      <c r="G39" t="s" s="5">
+        <v>82</v>
+      </c>
+      <c r="H39" t="s" s="5">
+        <v>83</v>
+      </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
@@ -2672,21 +2826,27 @@
     </row>
     <row r="40" ht="11.65" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="B40" t="s" s="3">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C40" t="s" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D40" t="s" s="3">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
+      <c r="F40" t="s" s="3">
+        <v>88</v>
+      </c>
+      <c r="G40" t="s" s="3">
+        <v>89</v>
+      </c>
+      <c r="H40" t="s" s="3">
+        <v>90</v>
+      </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -2695,19 +2855,27 @@
     </row>
     <row r="41" ht="11.65" customHeight="1">
       <c r="A41" t="s" s="5">
+        <v>132</v>
+      </c>
+      <c r="B41" t="s" s="5">
+        <v>100</v>
+      </c>
+      <c r="C41" t="s" s="5">
+        <v>101</v>
+      </c>
+      <c r="D41" t="s" s="6">
         <v>102</v>
       </c>
-      <c r="B41" t="s" s="5">
-        <v>103</v>
-      </c>
-      <c r="C41" t="s" s="5">
-        <v>104</v>
-      </c>
-      <c r="D41" s="2"/>
       <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
+      <c r="F41" t="s" s="5">
+        <v>119</v>
+      </c>
+      <c r="G41" t="s" s="5">
+        <v>120</v>
+      </c>
+      <c r="H41" t="s" s="5">
+        <v>133</v>
+      </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
@@ -2716,15 +2884,17 @@
     </row>
     <row r="42" ht="11.65" customHeight="1">
       <c r="A42" t="s" s="3">
+        <v>134</v>
+      </c>
+      <c r="B42" t="s" s="3">
+        <v>104</v>
+      </c>
+      <c r="C42" t="s" s="3">
         <v>105</v>
       </c>
-      <c r="B42" t="s" s="3">
+      <c r="D42" t="s" s="6">
         <v>106</v>
       </c>
-      <c r="C42" t="s" s="3">
-        <v>107</v>
-      </c>
-      <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -2737,16 +2907,16 @@
     </row>
     <row r="43" ht="11.65" customHeight="1">
       <c r="A43" t="s" s="5">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="B43" t="s" s="5">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s" s="5">
         <v>1</v>
       </c>
       <c r="D43" t="s" s="5">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
@@ -2760,16 +2930,16 @@
     </row>
     <row r="44" ht="11.65" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B44" t="s" s="3">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C44" t="s" s="3">
         <v>1</v>
       </c>
       <c r="D44" t="s" s="3">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -2783,7 +2953,7 @@
     </row>
     <row r="45" ht="11.65" customHeight="1">
       <c r="A45" t="s" s="5">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2800,16 +2970,16 @@
     </row>
     <row r="46" ht="11.65" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>101</v>
+        <v>137</v>
       </c>
       <c r="B46" t="s" s="3">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C46" t="s" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D46" t="s" s="3">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -2823,15 +2993,17 @@
     </row>
     <row r="47" ht="11.65" customHeight="1">
       <c r="A47" t="s" s="5">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="B47" t="s" s="5">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="C47" t="s" s="5">
-        <v>111</v>
-      </c>
-      <c r="D47" s="2"/>
+        <v>123</v>
+      </c>
+      <c r="D47" t="s" s="6">
+        <v>124</v>
+      </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -2844,15 +3016,17 @@
     </row>
     <row r="48" ht="11.65" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="B48" t="s" s="3">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="C48" t="s" s="3">
-        <v>113</v>
-      </c>
-      <c r="D48" s="4"/>
+        <v>128</v>
+      </c>
+      <c r="D48" t="s" s="6">
+        <v>129</v>
+      </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -2865,16 +3039,16 @@
     </row>
     <row r="49" ht="11.65" customHeight="1">
       <c r="A49" t="s" s="5">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="B49" t="s" s="5">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C49" t="s" s="5">
         <v>1</v>
       </c>
       <c r="D49" t="s" s="5">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -2888,16 +3062,16 @@
     </row>
     <row r="50" ht="11.65" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B50" t="s" s="3">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C50" t="s" s="3">
         <v>1</v>
       </c>
       <c r="D50" t="s" s="3">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
@@ -2911,7 +3085,7 @@
     </row>
     <row r="51" ht="11.65" customHeight="1">
       <c r="A51" t="s" s="5">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2928,16 +3102,16 @@
     </row>
     <row r="52" ht="11.65" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="B52" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C52" t="s" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D52" t="s" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
@@ -2951,16 +3125,16 @@
     </row>
     <row r="53" ht="11.65" customHeight="1">
       <c r="A53" t="s" s="5">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="B53" t="s" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C53" t="s" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D53" t="s" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
@@ -2974,16 +3148,16 @@
     </row>
     <row r="54" ht="11.65" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="B54" t="s" s="3">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C54" t="s" s="3">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D54" t="s" s="3">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -2997,7 +3171,7 @@
     </row>
     <row r="55" ht="11.65" customHeight="1">
       <c r="A55" t="s" s="5">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -3014,16 +3188,16 @@
     </row>
     <row r="56" ht="11.65" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="B56" t="s" s="3">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C56" t="s" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D56" t="s" s="3">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
@@ -3037,16 +3211,16 @@
     </row>
     <row r="57" ht="11.65" customHeight="1">
       <c r="A57" t="s" s="5">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="B57" t="s" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C57" t="s" s="5">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D57" t="s" s="5">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
@@ -3060,7 +3234,7 @@
     </row>
     <row r="58" ht="11.65" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -3077,16 +3251,16 @@
     </row>
     <row r="59" ht="11.65" customHeight="1">
       <c r="A59" t="s" s="5">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="B59" t="s" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C59" t="s" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D59" t="s" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
@@ -3100,16 +3274,16 @@
     </row>
     <row r="60" ht="11.65" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="B60" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C60" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D60" t="s" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
@@ -3123,16 +3297,16 @@
     </row>
     <row r="61" ht="11.65" customHeight="1">
       <c r="A61" t="s" s="5">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="B61" t="s" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C61" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D61" t="s" s="5">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
@@ -3146,16 +3320,16 @@
     </row>
     <row r="62" ht="11.65" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="B62" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C62" t="s" s="3">
         <v>1</v>
       </c>
       <c r="D62" t="s" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
@@ -3169,16 +3343,16 @@
     </row>
     <row r="63" ht="11.65" customHeight="1">
       <c r="A63" t="s" s="5">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="B63" t="s" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C63" t="s" s="5">
         <v>1</v>
       </c>
       <c r="D63" t="s" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
@@ -3192,15 +3366,17 @@
     </row>
     <row r="64" ht="11.65" customHeight="1">
       <c r="A64" t="s" s="3">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="B64" t="s" s="3">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C64" t="s" s="3">
-        <v>129</v>
-      </c>
-      <c r="D64" s="4"/>
+        <v>112</v>
+      </c>
+      <c r="D64" t="s" s="6">
+        <v>113</v>
+      </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -3213,15 +3389,17 @@
     </row>
     <row r="65" ht="11.65" customHeight="1">
       <c r="A65" t="s" s="5">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="B65" t="s" s="5">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="C65" t="s" s="5">
-        <v>132</v>
-      </c>
-      <c r="D65" s="2"/>
+        <v>116</v>
+      </c>
+      <c r="D65" t="s" s="6">
+        <v>117</v>
+      </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
@@ -3234,16 +3412,16 @@
     </row>
     <row r="66" ht="11.65" customHeight="1">
       <c r="A66" t="s" s="3">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="B66" t="s" s="3">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C66" t="s" s="3">
         <v>1</v>
       </c>
       <c r="D66" t="s" s="3">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
@@ -3257,16 +3435,16 @@
     </row>
     <row r="67" ht="11.65" customHeight="1">
       <c r="A67" t="s" s="5">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="B67" t="s" s="5">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C67" t="s" s="5">
         <v>1</v>
       </c>
       <c r="D67" t="s" s="5">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
@@ -3280,12 +3458,12 @@
     </row>
     <row r="68" ht="11.65" customHeight="1">
       <c r="A68" t="s" s="3">
-        <v>135</v>
-      </c>
-      <c r="B68" s="6">
+        <v>157</v>
+      </c>
+      <c r="B68" s="7">
         <v>1</v>
       </c>
-      <c r="C68" s="6">
+      <c r="C68" s="7">
         <v>0.7</v>
       </c>
       <c r="D68" s="4"/>
@@ -3301,7 +3479,7 @@
     </row>
     <row r="69" ht="11.65" customHeight="1">
       <c r="A69" t="s" s="5">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -3318,16 +3496,16 @@
     </row>
     <row r="70" ht="11.65" customHeight="1">
       <c r="A70" t="s" s="3">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="B70" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C70" t="s" s="3">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D70" t="s" s="3">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
@@ -3341,16 +3519,16 @@
     </row>
     <row r="71" ht="11.65" customHeight="1">
       <c r="A71" t="s" s="5">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="B71" t="s" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C71" t="s" s="5">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D71" t="s" s="5">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -3364,15 +3542,17 @@
     </row>
     <row r="72" ht="11.65" customHeight="1">
       <c r="A72" t="s" s="3">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="B72" t="s" s="3">
-        <v>140</v>
+        <v>84</v>
       </c>
       <c r="C72" t="s" s="3">
-        <v>140</v>
-      </c>
-      <c r="D72" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="D72" t="s" s="6">
+        <v>86</v>
+      </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
@@ -3384,16 +3564,10 @@
       <c r="M72" s="4"/>
     </row>
     <row r="73" ht="11.65" customHeight="1">
-      <c r="A73" t="s" s="5">
-        <v>141</v>
-      </c>
-      <c r="B73" t="s" s="5">
-        <v>142</v>
-      </c>
-      <c r="C73" t="s" s="5">
-        <v>142</v>
-      </c>
-      <c r="D73" s="2"/>
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="8"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
@@ -3406,16 +3580,16 @@
     </row>
     <row r="74" ht="11.65" customHeight="1">
       <c r="A74" t="s" s="3">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="B74" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C74" t="s" s="3">
         <v>1</v>
       </c>
       <c r="D74" t="s" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
@@ -3429,16 +3603,16 @@
     </row>
     <row r="75" ht="11.65" customHeight="1">
       <c r="A75" t="s" s="5">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="B75" t="s" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C75" t="s" s="5">
         <v>1</v>
       </c>
       <c r="D75" t="s" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
@@ -3452,16 +3626,16 @@
     </row>
     <row r="76" ht="11.65" customHeight="1">
       <c r="A76" t="s" s="3">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="B76" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C76" t="s" s="3">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D76" t="s" s="3">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
@@ -3475,16 +3649,16 @@
     </row>
     <row r="77" ht="11.65" customHeight="1">
       <c r="A77" t="s" s="5">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="B77" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C77" t="s" s="5">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D77" t="s" s="5">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -3498,7 +3672,7 @@
     </row>
     <row r="78" ht="11.65" customHeight="1">
       <c r="A78" t="s" s="3">
-        <v>145</v>
+        <v>164</v>
       </c>
       <c r="B78" t="s" s="3">
         <v>1</v>
@@ -3507,7 +3681,7 @@
         <v>1</v>
       </c>
       <c r="D78" t="s" s="3">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -3521,7 +3695,7 @@
     </row>
     <row r="79" ht="11.65" customHeight="1">
       <c r="A79" t="s" s="5">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -3538,16 +3712,16 @@
     </row>
     <row r="80" ht="11.65" customHeight="1">
       <c r="A80" t="s" s="3">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="B80" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C80" t="s" s="3">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D80" t="s" s="3">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
@@ -3561,13 +3735,13 @@
     </row>
     <row r="81" ht="11.65" customHeight="1">
       <c r="A81" t="s" s="5">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="B81" t="s" s="5">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="C81" t="s" s="5">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -3582,15 +3756,17 @@
     </row>
     <row r="82" ht="11.65" customHeight="1">
       <c r="A82" t="s" s="3">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="B82" t="s" s="3">
-        <v>151</v>
+        <v>108</v>
       </c>
       <c r="C82" t="s" s="3">
-        <v>151</v>
-      </c>
-      <c r="D82" s="4"/>
+        <v>108</v>
+      </c>
+      <c r="D82" t="s" s="6">
+        <v>109</v>
+      </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
@@ -3603,13 +3779,13 @@
     </row>
     <row r="83" ht="11.65" customHeight="1">
       <c r="A83" t="s" s="5">
-        <v>152</v>
-      </c>
-      <c r="B83" s="7">
+        <v>170</v>
+      </c>
+      <c r="B83" s="9">
         <v>1</v>
       </c>
       <c r="C83" t="s" s="5">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -3624,16 +3800,16 @@
     </row>
     <row r="84" ht="11.65" customHeight="1">
       <c r="A84" t="s" s="3">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="B84" t="s" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C84" t="s" s="3">
         <v>1</v>
       </c>
       <c r="D84" t="s" s="3">
-        <v>155</v>
+        <v>39</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
@@ -3647,13 +3823,13 @@
     </row>
     <row r="85" ht="11.65" customHeight="1">
       <c r="A85" t="s" s="5">
-        <v>156</v>
-      </c>
-      <c r="B85" s="7">
+        <v>173</v>
+      </c>
+      <c r="B85" s="9">
         <v>1</v>
       </c>
       <c r="C85" t="s" s="5">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
@@ -3668,16 +3844,16 @@
     </row>
     <row r="86" ht="11.65" customHeight="1">
       <c r="A86" t="s" s="3">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="B86" t="s" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C86" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D86" t="s" s="3">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>

</xml_diff>